<commit_message>
Added my two user stories
</commit_message>
<xml_diff>
--- a/TeamVOXSReport.xlsx
+++ b/TeamVOXSReport.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/smallv/Documents/GitHub/SSW-555/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6D677C2-DF3B-F84E-877C-C23B5EAA6A69}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13B22A98-FE55-3246-A6AF-3445DD1DA683}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14560" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14560" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="228">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -770,6 +770,10 @@
   </si>
   <si>
     <t>No more than five siblings should be born at the same time</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Yes</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -925,7 +929,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -955,6 +959,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="65"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="176" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="66">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -2112,7 +2117,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+    <sheetView topLeftCell="A11" zoomScale="150" workbookViewId="0">
       <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
@@ -2120,7 +2125,7 @@
   <cols>
     <col min="1" max="1" width="8.83203125" customWidth="1"/>
     <col min="2" max="2" width="23.5" customWidth="1"/>
-    <col min="3" max="3" width="52.83203125" customWidth="1"/>
+    <col min="3" max="3" width="82.5" customWidth="1"/>
     <col min="4" max="4" width="24.83203125" customWidth="1"/>
     <col min="5" max="5" width="20.83203125" customWidth="1"/>
     <col min="6" max="6" width="26.83203125" customWidth="1"/>
@@ -3098,8 +3103,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" zoomScale="150" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13"/>
@@ -3371,8 +3376,8 @@
       <c r="H9">
         <v>20</v>
       </c>
-      <c r="I9" s="7" t="s">
-        <v>203</v>
+      <c r="I9" s="19" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -3459,7 +3464,7 @@
       <c r="A14" t="s">
         <v>120</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="1" t="s">
         <v>207</v>
       </c>
       <c r="C14" t="s">
@@ -3473,13 +3478,22 @@
       </c>
       <c r="F14">
         <v>80</v>
+      </c>
+      <c r="G14">
+        <v>30</v>
+      </c>
+      <c r="H14">
+        <v>50</v>
+      </c>
+      <c r="I14" s="19" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="14">
       <c r="A15" t="s">
         <v>121</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="1" t="s">
         <v>165</v>
       </c>
       <c r="C15" t="s">
@@ -3494,13 +3508,21 @@
       <c r="F15">
         <v>80</v>
       </c>
-      <c r="I15" s="7"/>
+      <c r="G15">
+        <v>30</v>
+      </c>
+      <c r="H15">
+        <v>50</v>
+      </c>
+      <c r="I15" s="19" t="s">
+        <v>227</v>
+      </c>
     </row>
     <row r="16" spans="1:9" ht="14">
       <c r="A16" t="s">
         <v>122</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B16" s="1" t="s">
         <v>93</v>
       </c>
       <c r="C16" t="s">
@@ -3582,6 +3604,9 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13"/>
+  <cols>
+    <col min="2" max="2" width="24.5" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="28">
       <c r="A1" s="4" t="s">

</xml_diff>

<commit_message>
update report and sprint 2 output
</commit_message>
<xml_diff>
--- a/TeamVOXSReport.xlsx
+++ b/TeamVOXSReport.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10910"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20827"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/smallv/Documents/GitHub/SSW-555/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MS SE\SSW-555\Sanjeev Branch\SSW-555\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6D677C2-DF3B-F84E-877C-C23B5EAA6A69}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5401F60B-F0A7-4003-BFE2-347C4C25023C}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14560" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="25605" windowHeight="14565" tabRatio="500" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
     <sheet name="Sprint4" sheetId="6" r:id="rId8"/>
     <sheet name="Stories" sheetId="11" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="179021" concurrentCalc="0"/>
+  <calcPr calcId="162913" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="557" uniqueCount="230">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -515,9 +515,6 @@
   </si>
   <si>
     <t>US42</t>
-  </si>
-  <si>
-    <t>Coding</t>
   </si>
   <si>
     <t>Dates before current date</t>
@@ -772,14 +769,26 @@
     <t>No more than five siblings should be born at the same time</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
+  <si>
+    <t>Use Github Better</t>
+  </si>
+  <si>
+    <t>Learn to use Travis</t>
+  </si>
+  <si>
+    <t>Not using Github</t>
+  </si>
+  <si>
+    <t>Coding</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="176" formatCode="m/d"/>
-    <numFmt numFmtId="177" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="m/d"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
   <fonts count="9">
     <font>
@@ -930,20 +939,20 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -951,78 +960,78 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="177" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="65"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="66">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="超链接" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="13" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="15" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="17" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="19" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="21" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="23" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="25" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="27" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="29" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="31" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="33" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="35" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="37" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="39" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="41" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="43" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="45" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="47" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="49" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="51" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="53" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="55" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="57" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="59" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="61" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="63" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="65" builtinId="8"/>
-    <cellStyle name="已访问的超链接" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="22" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="24" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="26" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="28" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="30" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="32" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="34" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="36" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="38" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="40" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="42" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="44" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="46" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="48" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="50" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="52" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="54" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="56" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="58" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="60" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="62" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -1040,7 +1049,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="1"/>
-  <c:lang val="zh-CN"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1064,7 +1073,7 @@
             <c:numRef>
               <c:f>'Burndown README'!$B$15:$B$20</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yy</c:formatCode>
+                <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>41065</c:v>
@@ -1135,7 +1144,7 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="m/d/yy" sourceLinked="1"/>
+        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1177,7 +1186,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="1"/>
-  <c:lang val="zh-CN"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1209,6 +1218,9 @@
                 <c:pt idx="1">
                   <c:v>41917</c:v>
                 </c:pt>
+                <c:pt idx="2">
+                  <c:v>41805</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -1223,6 +1235,9 @@
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2110,21 +2125,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G29"/>
+  <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView topLeftCell="A36" zoomScale="150" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13:B37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="8.83203125" customWidth="1"/>
+    <col min="1" max="1" width="8.875" customWidth="1"/>
     <col min="2" max="2" width="23.5" customWidth="1"/>
-    <col min="3" max="3" width="52.83203125" customWidth="1"/>
-    <col min="4" max="4" width="24.83203125" customWidth="1"/>
-    <col min="5" max="5" width="20.83203125" customWidth="1"/>
-    <col min="6" max="6" width="26.83203125" customWidth="1"/>
-    <col min="7" max="7" width="22.33203125" customWidth="1"/>
+    <col min="3" max="3" width="52.875" customWidth="1"/>
+    <col min="4" max="4" width="24.875" customWidth="1"/>
+    <col min="5" max="5" width="20.875" customWidth="1"/>
+    <col min="6" max="6" width="26.875" customWidth="1"/>
+    <col min="7" max="7" width="22.375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="4" customFormat="1">
@@ -2135,7 +2150,7 @@
         <v>20</v>
       </c>
       <c r="C1" s="18" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>21</v>
@@ -2146,75 +2161,75 @@
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
+        <v>171</v>
+      </c>
+      <c r="B3" t="s">
         <v>172</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" s="17" t="s">
         <v>173</v>
       </c>
-      <c r="C3" s="17" t="s">
+      <c r="D3" s="16" t="s">
         <v>174</v>
       </c>
-      <c r="D3" s="16" t="s">
-        <v>175</v>
-      </c>
       <c r="E3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
+        <v>175</v>
+      </c>
+      <c r="B4" t="s">
         <v>176</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" s="17" t="s">
         <v>177</v>
       </c>
-      <c r="C4" s="17" t="s">
+      <c r="D4" s="16" t="s">
         <v>178</v>
       </c>
-      <c r="D4" s="16" t="s">
-        <v>179</v>
-      </c>
       <c r="E4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="17" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B5" t="s">
+        <v>179</v>
+      </c>
+      <c r="C5" s="17" t="s">
         <v>180</v>
       </c>
-      <c r="C5" s="17" t="s">
+      <c r="D5" s="16" t="s">
         <v>181</v>
       </c>
-      <c r="D5" s="16" t="s">
-        <v>182</v>
-      </c>
       <c r="E5" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="17" t="s">
+        <v>217</v>
+      </c>
+      <c r="B6" s="17" t="s">
         <v>218</v>
       </c>
-      <c r="B6" s="17" t="s">
+      <c r="C6" s="17" t="s">
         <v>219</v>
       </c>
-      <c r="C6" s="17" t="s">
+      <c r="D6" s="16" t="s">
         <v>220</v>
       </c>
-      <c r="D6" s="16" t="s">
+      <c r="E6" s="17" t="s">
         <v>221</v>
-      </c>
-      <c r="E6" s="17" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="C7" s="17" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -2232,16 +2247,16 @@
         <v>61</v>
       </c>
       <c r="D11" s="18" t="s">
+        <v>182</v>
+      </c>
+      <c r="E11" s="18" t="s">
         <v>183</v>
       </c>
-      <c r="E11" s="18" t="s">
-        <v>184</v>
-      </c>
       <c r="F11" s="18" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="G11" s="18" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -2252,10 +2267,10 @@
         <v>82</v>
       </c>
       <c r="C13" s="17" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D13" s="17" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E13">
         <v>120</v>
@@ -2264,7 +2279,7 @@
         <v>130</v>
       </c>
       <c r="G13" s="17" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -2275,10 +2290,10 @@
         <v>66</v>
       </c>
       <c r="C14" s="17" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D14" s="17" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E14">
         <v>90</v>
@@ -2287,7 +2302,7 @@
         <v>100</v>
       </c>
       <c r="G14" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -2298,10 +2313,10 @@
         <v>77</v>
       </c>
       <c r="C15" s="17" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D15" s="17" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E15">
         <v>110</v>
@@ -2310,7 +2325,7 @@
         <v>150</v>
       </c>
       <c r="G15" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -2321,10 +2336,10 @@
         <v>94</v>
       </c>
       <c r="C16" s="17" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D16" s="17" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E16">
         <v>140</v>
@@ -2333,7 +2348,7 @@
         <v>180</v>
       </c>
       <c r="G16" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -2344,10 +2359,10 @@
         <v>67</v>
       </c>
       <c r="C17" s="17" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D17" s="17" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E17">
         <v>80</v>
@@ -2356,7 +2371,7 @@
         <v>100</v>
       </c>
       <c r="G17" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -2367,10 +2382,10 @@
         <v>71</v>
       </c>
       <c r="C18" s="17" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D18" s="17" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E18">
         <v>90</v>
@@ -2379,7 +2394,7 @@
         <v>105</v>
       </c>
       <c r="G18" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -2390,10 +2405,10 @@
         <v>79</v>
       </c>
       <c r="C19" s="17" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D19" s="17" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E19">
         <v>100</v>
@@ -2402,7 +2417,7 @@
         <v>120</v>
       </c>
       <c r="G19" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -2413,10 +2428,10 @@
         <v>85</v>
       </c>
       <c r="C20" s="17" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D20" s="17" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E20">
         <v>90</v>
@@ -2425,7 +2440,7 @@
         <v>110</v>
       </c>
       <c r="G20" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -2436,10 +2451,10 @@
         <v>76</v>
       </c>
       <c r="C21" s="17" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D21" s="17" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E21">
         <v>80</v>
@@ -2448,7 +2463,7 @@
         <v>120</v>
       </c>
       <c r="G21" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -2456,13 +2471,13 @@
         <v>117</v>
       </c>
       <c r="B22" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C22" s="17" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D22" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E22">
         <v>30</v>
@@ -2476,13 +2491,13 @@
         <v>118</v>
       </c>
       <c r="B23" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C23" s="17" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D23" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E23">
         <v>30</v>
@@ -2496,13 +2511,13 @@
         <v>119</v>
       </c>
       <c r="B24" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C24" s="17" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D24" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E24">
         <v>30</v>
@@ -2519,10 +2534,10 @@
         <v>63</v>
       </c>
       <c r="C25" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D25" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E25">
         <v>30</v>
@@ -2536,13 +2551,13 @@
         <v>121</v>
       </c>
       <c r="B26" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C26" s="17" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D26" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E26">
         <v>30</v>
@@ -2556,13 +2571,13 @@
         <v>122</v>
       </c>
       <c r="B27" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C27" s="17" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D27" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E27">
         <v>30</v>
@@ -2579,7 +2594,7 @@
         <v>93</v>
       </c>
       <c r="D28" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E28">
         <v>30</v>
@@ -2593,16 +2608,128 @@
         <v>124</v>
       </c>
       <c r="B29" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D29" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E29">
         <v>30</v>
       </c>
       <c r="F29">
         <v>80</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="15.75">
+      <c r="A30" t="s">
+        <v>125</v>
+      </c>
+      <c r="B30" t="s">
+        <v>78</v>
+      </c>
+      <c r="C30" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="D30" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="15.75">
+      <c r="A31" t="s">
+        <v>126</v>
+      </c>
+      <c r="B31" t="s">
+        <v>79</v>
+      </c>
+      <c r="C31" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="D31" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="15.75">
+      <c r="A32" t="s">
+        <v>127</v>
+      </c>
+      <c r="B32" t="s">
+        <v>80</v>
+      </c>
+      <c r="C32" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="D32" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="31.5">
+      <c r="A33" t="s">
+        <v>128</v>
+      </c>
+      <c r="B33" t="s">
+        <v>81</v>
+      </c>
+      <c r="C33" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="D33" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="31.5">
+      <c r="A34" t="s">
+        <v>129</v>
+      </c>
+      <c r="B34" t="s">
+        <v>82</v>
+      </c>
+      <c r="C34" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="D34" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="31.5">
+      <c r="A35" t="s">
+        <v>130</v>
+      </c>
+      <c r="B35" t="s">
+        <v>85</v>
+      </c>
+      <c r="C35" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="D35" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="31.5">
+      <c r="A36" t="s">
+        <v>131</v>
+      </c>
+      <c r="B36" t="s">
+        <v>86</v>
+      </c>
+      <c r="C36" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="D36" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="47.25">
+      <c r="A37" t="s">
+        <v>132</v>
+      </c>
+      <c r="B37" t="s">
+        <v>87</v>
+      </c>
+      <c r="C37" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="D37" t="s">
+        <v>199</v>
       </c>
     </row>
   </sheetData>
@@ -2623,19 +2750,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E10"/>
+    <sheetView topLeftCell="A13" zoomScale="150" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19:E26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="5.1640625" customWidth="1"/>
-    <col min="2" max="2" width="7.6640625" customWidth="1"/>
-    <col min="3" max="3" width="24.1640625" customWidth="1"/>
-    <col min="4" max="4" width="9.1640625" customWidth="1"/>
-    <col min="5" max="5" width="7.6640625" customWidth="1"/>
+    <col min="1" max="1" width="5.125" customWidth="1"/>
+    <col min="2" max="2" width="7.625" customWidth="1"/>
+    <col min="3" max="3" width="24.125" customWidth="1"/>
+    <col min="4" max="4" width="9.125" customWidth="1"/>
+    <col min="5" max="5" width="7.625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="4" customFormat="1">
@@ -2666,10 +2793,10 @@
         <v>82</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -2683,15 +2810,15 @@
         <v>66</v>
       </c>
       <c r="D3" s="17" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B4" t="s">
         <v>110</v>
@@ -2700,15 +2827,15 @@
         <v>77</v>
       </c>
       <c r="D4" s="17" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E4" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B5" t="s">
         <v>111</v>
@@ -2717,15 +2844,15 @@
         <v>94</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E5" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B6" t="s">
         <v>112</v>
@@ -2734,15 +2861,15 @@
         <v>67</v>
       </c>
       <c r="D6" s="17" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E6" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B7" t="s">
         <v>113</v>
@@ -2751,15 +2878,15 @@
         <v>71</v>
       </c>
       <c r="D7" s="17" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E7" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="B8" t="s">
         <v>114</v>
@@ -2768,15 +2895,15 @@
         <v>79</v>
       </c>
       <c r="D8" s="17" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E8" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="B9" t="s">
         <v>115</v>
@@ -2785,15 +2912,15 @@
         <v>85</v>
       </c>
       <c r="D9" s="17" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E9" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="B10" s="17" t="s">
         <v>116</v>
@@ -2802,10 +2929,282 @@
         <v>76</v>
       </c>
       <c r="D10" s="17" t="s">
+        <v>199</v>
+      </c>
+      <c r="E10" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11">
+        <v>2</v>
+      </c>
+      <c r="B11" t="s">
+        <v>117</v>
+      </c>
+      <c r="C11" t="s">
+        <v>203</v>
+      </c>
+      <c r="D11" s="17" t="s">
+        <v>171</v>
+      </c>
+      <c r="E11" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12">
+        <v>2</v>
+      </c>
+      <c r="B12" t="s">
+        <v>118</v>
+      </c>
+      <c r="C12" t="s">
+        <v>204</v>
+      </c>
+      <c r="D12" s="17" t="s">
+        <v>171</v>
+      </c>
+      <c r="E12" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13">
+        <v>2</v>
+      </c>
+      <c r="B13" t="s">
+        <v>119</v>
+      </c>
+      <c r="C13" t="s">
+        <v>205</v>
+      </c>
+      <c r="D13" s="17" t="s">
         <v>200</v>
       </c>
-      <c r="E10" t="s">
-        <v>202</v>
+      <c r="E13" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14">
+        <v>2</v>
+      </c>
+      <c r="B14" t="s">
+        <v>120</v>
+      </c>
+      <c r="C14" t="s">
+        <v>63</v>
+      </c>
+      <c r="D14" s="17" t="s">
+        <v>200</v>
+      </c>
+      <c r="E14" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15">
+        <v>2</v>
+      </c>
+      <c r="B15" t="s">
+        <v>121</v>
+      </c>
+      <c r="C15" t="s">
+        <v>206</v>
+      </c>
+      <c r="D15" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="E15" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16">
+        <v>2</v>
+      </c>
+      <c r="B16" t="s">
+        <v>122</v>
+      </c>
+      <c r="C16" t="s">
+        <v>164</v>
+      </c>
+      <c r="D16" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="E16" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17">
+        <v>2</v>
+      </c>
+      <c r="B17" t="s">
+        <v>123</v>
+      </c>
+      <c r="C17" t="s">
+        <v>93</v>
+      </c>
+      <c r="D17" s="17" t="s">
+        <v>199</v>
+      </c>
+      <c r="E17" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18">
+        <v>2</v>
+      </c>
+      <c r="B18" t="s">
+        <v>124</v>
+      </c>
+      <c r="C18" t="s">
+        <v>150</v>
+      </c>
+      <c r="D18" s="17" t="s">
+        <v>199</v>
+      </c>
+      <c r="E18" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19">
+        <v>3</v>
+      </c>
+      <c r="B19" t="s">
+        <v>125</v>
+      </c>
+      <c r="C19" t="s">
+        <v>78</v>
+      </c>
+      <c r="D19" s="17" t="s">
+        <v>171</v>
+      </c>
+      <c r="E19" s="17" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20">
+        <v>3</v>
+      </c>
+      <c r="B20" t="s">
+        <v>126</v>
+      </c>
+      <c r="C20" t="s">
+        <v>79</v>
+      </c>
+      <c r="D20" s="17" t="s">
+        <v>171</v>
+      </c>
+      <c r="E20" s="17" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21">
+        <v>3</v>
+      </c>
+      <c r="B21" t="s">
+        <v>127</v>
+      </c>
+      <c r="C21" t="s">
+        <v>80</v>
+      </c>
+      <c r="D21" s="17" t="s">
+        <v>200</v>
+      </c>
+      <c r="E21" s="17" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22">
+        <v>3</v>
+      </c>
+      <c r="B22" t="s">
+        <v>128</v>
+      </c>
+      <c r="C22" t="s">
+        <v>81</v>
+      </c>
+      <c r="D22" s="17" t="s">
+        <v>200</v>
+      </c>
+      <c r="E22" s="17" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23">
+        <v>3</v>
+      </c>
+      <c r="B23" t="s">
+        <v>129</v>
+      </c>
+      <c r="C23" t="s">
+        <v>82</v>
+      </c>
+      <c r="D23" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="E23" s="17" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24">
+        <v>3</v>
+      </c>
+      <c r="B24" t="s">
+        <v>130</v>
+      </c>
+      <c r="C24" t="s">
+        <v>85</v>
+      </c>
+      <c r="D24" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="E24" s="17" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25">
+        <v>3</v>
+      </c>
+      <c r="B25" t="s">
+        <v>131</v>
+      </c>
+      <c r="C25" t="s">
+        <v>86</v>
+      </c>
+      <c r="D25" s="17" t="s">
+        <v>199</v>
+      </c>
+      <c r="E25" s="17" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26">
+        <v>3</v>
+      </c>
+      <c r="B26" t="s">
+        <v>132</v>
+      </c>
+      <c r="C26" t="s">
+        <v>87</v>
+      </c>
+      <c r="D26" s="17" t="s">
+        <v>199</v>
+      </c>
+      <c r="E26" s="17" t="s">
+        <v>229</v>
       </c>
     </row>
   </sheetData>
@@ -2823,49 +3222,49 @@
       <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="7"/>
+    <col min="1" max="1" width="10.875" style="7"/>
     <col min="2" max="2" width="9.5" customWidth="1"/>
-    <col min="3" max="3" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.33203125" customWidth="1"/>
-    <col min="5" max="5" width="6.83203125" customWidth="1"/>
+    <col min="3" max="3" width="15.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.375" customWidth="1"/>
+    <col min="5" max="5" width="6.875" customWidth="1"/>
     <col min="6" max="6" width="12.5" style="9" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="7" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="7" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="7" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="7" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="7" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="14" spans="1:7" s="4" customFormat="1">
       <c r="A14" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>0</v>
@@ -2888,7 +3287,7 @@
     </row>
     <row r="15" spans="1:7">
       <c r="A15" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B15" s="13">
         <v>41065</v>
@@ -2904,7 +3303,7 @@
     </row>
     <row r="16" spans="1:7">
       <c r="A16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B16" s="13">
         <v>41078</v>
@@ -2929,7 +3328,7 @@
     </row>
     <row r="17" spans="1:7">
       <c r="A17" s="7" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B17" s="13">
         <v>41092</v>
@@ -2954,7 +3353,7 @@
     </row>
     <row r="18" spans="1:7">
       <c r="A18" s="7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B18" s="13">
         <v>41106</v>
@@ -2979,7 +3378,7 @@
     </row>
     <row r="19" spans="1:7">
       <c r="A19" s="7" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B19" s="13">
         <v>41120</v>
@@ -3012,19 +3411,19 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="2"/>
-    <col min="2" max="2" width="16.6640625" customWidth="1"/>
+    <col min="1" max="1" width="10.875" style="2"/>
+    <col min="2" max="2" width="16.625" customWidth="1"/>
     <col min="3" max="3" width="12.5" customWidth="1"/>
-    <col min="4" max="4" width="7.1640625" customWidth="1"/>
-    <col min="5" max="5" width="6.83203125" customWidth="1"/>
+    <col min="4" max="4" width="7.125" customWidth="1"/>
+    <col min="5" max="5" width="6.875" customWidth="1"/>
     <col min="6" max="6" width="12.5" style="9" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3055,9 +3454,6 @@
       <c r="B2">
         <v>32</v>
       </c>
-      <c r="C2">
-        <v>60</v>
-      </c>
       <c r="D2">
         <v>0</v>
       </c>
@@ -3073,7 +3469,7 @@
         <v>24</v>
       </c>
       <c r="C3">
-        <v>50</v>
+        <v>8</v>
       </c>
       <c r="D3">
         <v>317</v>
@@ -3084,6 +3480,27 @@
       <c r="F3" s="9">
         <f>(D3-D2)/E3*60</f>
         <v>82.695652173913047</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="2">
+        <v>41805</v>
+      </c>
+      <c r="B4">
+        <v>16</v>
+      </c>
+      <c r="C4">
+        <v>8</v>
+      </c>
+      <c r="D4">
+        <v>365</v>
+      </c>
+      <c r="E4">
+        <v>150</v>
+      </c>
+      <c r="F4" s="9">
+        <f>(D4-D3)/E4*60</f>
+        <v>19.2</v>
       </c>
     </row>
   </sheetData>
@@ -3096,25 +3513,25 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:I26"/>
+  <dimension ref="A1:I18"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" zoomScale="150" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView topLeftCell="A4" zoomScale="150" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="7.6640625" customWidth="1"/>
+    <col min="1" max="1" width="7.625" customWidth="1"/>
     <col min="2" max="2" width="24.5" style="1" customWidth="1"/>
-    <col min="3" max="3" width="6.6640625" customWidth="1"/>
-    <col min="5" max="5" width="11.1640625" customWidth="1"/>
-    <col min="6" max="6" width="10.33203125" customWidth="1"/>
-    <col min="7" max="7" width="10.6640625" customWidth="1"/>
-    <col min="8" max="8" width="9.1640625" customWidth="1"/>
-    <col min="9" max="9" width="12.33203125" style="6" customWidth="1"/>
+    <col min="3" max="3" width="6.625" customWidth="1"/>
+    <col min="5" max="5" width="11.125" customWidth="1"/>
+    <col min="6" max="6" width="10.375" customWidth="1"/>
+    <col min="7" max="7" width="10.625" customWidth="1"/>
+    <col min="8" max="8" width="9.125" customWidth="1"/>
+    <col min="9" max="9" width="12.375" style="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="14">
+    <row r="1" spans="1:9">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -3151,10 +3568,10 @@
         <v>82</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E2">
         <v>15</v>
@@ -3169,7 +3586,7 @@
         <v>90</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -3180,10 +3597,10 @@
         <v>66</v>
       </c>
       <c r="C3" s="17" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E3">
         <v>10</v>
@@ -3198,7 +3615,7 @@
         <v>30</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -3209,10 +3626,10 @@
         <v>77</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D4" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E4">
         <v>20</v>
@@ -3227,7 +3644,7 @@
         <v>40</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -3238,10 +3655,10 @@
         <v>94</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D5" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E5">
         <v>40</v>
@@ -3256,7 +3673,7 @@
         <v>10</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -3267,10 +3684,10 @@
         <v>67</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D6" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E6">
         <v>20</v>
@@ -3285,7 +3702,7 @@
         <v>10</v>
       </c>
       <c r="I6" s="7" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -3296,10 +3713,10 @@
         <v>71</v>
       </c>
       <c r="C7" s="17" t="s">
+        <v>200</v>
+      </c>
+      <c r="D7" t="s">
         <v>201</v>
-      </c>
-      <c r="D7" t="s">
-        <v>202</v>
       </c>
       <c r="E7">
         <v>30</v>
@@ -3314,7 +3731,7 @@
         <v>15</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -3325,16 +3742,16 @@
         <v>79</v>
       </c>
       <c r="C8" s="17" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D8" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E8">
         <v>40</v>
       </c>
       <c r="F8">
-        <v>120</v>
+        <v>20</v>
       </c>
       <c r="G8">
         <v>10</v>
@@ -3343,7 +3760,7 @@
         <v>15</v>
       </c>
       <c r="I8" s="7" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -3354,16 +3771,16 @@
         <v>85</v>
       </c>
       <c r="C9" s="17" t="s">
+        <v>200</v>
+      </c>
+      <c r="D9" t="s">
         <v>201</v>
-      </c>
-      <c r="D9" t="s">
-        <v>202</v>
       </c>
       <c r="E9">
         <v>30</v>
       </c>
       <c r="F9">
-        <v>80</v>
+        <v>30</v>
       </c>
       <c r="G9">
         <v>10</v>
@@ -3372,198 +3789,37 @@
         <v>20</v>
       </c>
       <c r="I9" s="7" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9">
-      <c r="A10" s="17" t="s">
-        <v>116</v>
-      </c>
-      <c r="B10" s="17" t="s">
-        <v>204</v>
-      </c>
-      <c r="C10" s="17" t="s">
-        <v>172</v>
-      </c>
-      <c r="D10" t="s">
-        <v>150</v>
-      </c>
-      <c r="E10">
-        <v>30</v>
-      </c>
-      <c r="F10">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="14">
-      <c r="A11" t="s">
-        <v>117</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="C11" t="s">
-        <v>172</v>
-      </c>
-      <c r="D11" t="s">
-        <v>150</v>
-      </c>
-      <c r="E11">
-        <v>30</v>
-      </c>
-      <c r="F11">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="14">
-      <c r="A12" t="s">
-        <v>118</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="C12" t="s">
-        <v>176</v>
-      </c>
-      <c r="D12" t="s">
-        <v>150</v>
-      </c>
-      <c r="E12">
-        <v>30</v>
-      </c>
-      <c r="F12">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="14">
-      <c r="A13" t="s">
-        <v>119</v>
-      </c>
+        <v>202</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="B12" s="5" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
       <c r="B13" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="C13" t="s">
-        <v>176</v>
-      </c>
-      <c r="D13" t="s">
-        <v>150</v>
-      </c>
-      <c r="E13">
-        <v>30</v>
-      </c>
-      <c r="F13">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="14">
-      <c r="A14" t="s">
-        <v>120</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>207</v>
-      </c>
-      <c r="C14" t="s">
-        <v>201</v>
-      </c>
-      <c r="D14" t="s">
-        <v>150</v>
-      </c>
-      <c r="E14">
-        <v>30</v>
-      </c>
-      <c r="F14">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="14">
-      <c r="A15" t="s">
-        <v>121</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>165</v>
-      </c>
-      <c r="C15" t="s">
-        <v>201</v>
-      </c>
-      <c r="D15" t="s">
-        <v>150</v>
-      </c>
-      <c r="E15">
-        <v>30</v>
-      </c>
-      <c r="F15">
-        <v>80</v>
-      </c>
-      <c r="I15" s="7"/>
-    </row>
-    <row r="16" spans="1:9" ht="14">
-      <c r="A16" t="s">
-        <v>122</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="C16" t="s">
-        <v>200</v>
-      </c>
-      <c r="D16" t="s">
-        <v>150</v>
-      </c>
-      <c r="E16">
-        <v>30</v>
-      </c>
-      <c r="F16">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="14">
-      <c r="A17" t="s">
-        <v>123</v>
-      </c>
+        <v>213</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="B14" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="B16" s="1" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2">
       <c r="B17" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="C17" t="s">
-        <v>200</v>
-      </c>
-      <c r="D17" t="s">
-        <v>150</v>
-      </c>
-      <c r="E17">
-        <v>30</v>
-      </c>
-      <c r="F17">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="14">
-      <c r="B20" s="5" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="14">
-      <c r="B21" s="1" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="14">
-      <c r="B22" s="1" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="14">
-      <c r="B24" s="1" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="14">
-      <c r="B25" s="1" t="s">
+    <row r="18" spans="2:2" ht="25.5">
+      <c r="B18" s="1" t="s">
         <v>216</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="28">
-      <c r="B26" s="1" t="s">
-        <v>217</v>
       </c>
     </row>
   </sheetData>
@@ -3575,15 +3831,15 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:I18"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView topLeftCell="A16" zoomScale="150" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="28">
+    <row r="1" spans="1:9" ht="25.5">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -3613,163 +3869,260 @@
       </c>
     </row>
     <row r="2" spans="1:9">
-      <c r="A2" t="s">
+      <c r="A2" s="17" t="s">
         <v>116</v>
       </c>
-      <c r="B2" t="s">
-        <v>204</v>
-      </c>
-      <c r="C2" t="s">
-        <v>172</v>
+      <c r="B2" s="17" t="s">
+        <v>203</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>171</v>
       </c>
       <c r="D2" t="s">
-        <v>150</v>
+        <v>201</v>
       </c>
       <c r="E2">
+        <v>20</v>
+      </c>
+      <c r="F2">
+        <v>15</v>
+      </c>
+      <c r="G2">
         <v>30</v>
       </c>
-      <c r="F2">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
+      <c r="H2">
+        <v>20</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="38.25">
       <c r="A3" t="s">
         <v>117</v>
       </c>
-      <c r="B3" t="s">
-        <v>205</v>
+      <c r="B3" s="1" t="s">
+        <v>204</v>
       </c>
       <c r="C3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D3" t="s">
-        <v>150</v>
+        <v>201</v>
       </c>
       <c r="E3">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="F3">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
+        <v>10</v>
+      </c>
+      <c r="G3">
+        <v>20</v>
+      </c>
+      <c r="H3">
+        <v>10</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="38.25">
       <c r="A4" t="s">
         <v>118</v>
       </c>
-      <c r="B4" t="s">
-        <v>206</v>
+      <c r="B4" s="1" t="s">
+        <v>205</v>
       </c>
       <c r="C4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D4" t="s">
-        <v>150</v>
+        <v>201</v>
       </c>
       <c r="E4">
         <v>30</v>
       </c>
       <c r="F4">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
+        <v>15</v>
+      </c>
+      <c r="G4">
+        <v>30</v>
+      </c>
+      <c r="H4">
+        <v>20</v>
+      </c>
+      <c r="I4" s="7" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="25.5">
       <c r="A5" t="s">
         <v>119</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
         <v>73</v>
       </c>
       <c r="C5" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D5" t="s">
-        <v>150</v>
+        <v>201</v>
       </c>
       <c r="E5">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="F5">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
+        <v>25</v>
+      </c>
+      <c r="G5">
+        <v>20</v>
+      </c>
+      <c r="H5">
+        <v>25</v>
+      </c>
+      <c r="I5" s="7" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="25.5">
       <c r="A6" t="s">
         <v>120</v>
       </c>
-      <c r="B6" t="s">
-        <v>207</v>
+      <c r="B6" s="5" t="s">
+        <v>206</v>
       </c>
       <c r="C6" t="s">
+        <v>200</v>
+      </c>
+      <c r="D6" t="s">
         <v>201</v>
       </c>
-      <c r="D6" t="s">
-        <v>150</v>
-      </c>
       <c r="E6">
+        <v>20</v>
+      </c>
+      <c r="F6">
+        <v>15</v>
+      </c>
+      <c r="G6">
+        <v>25</v>
+      </c>
+      <c r="H6">
         <v>30</v>
       </c>
-      <c r="F6">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
+      <c r="I6" s="7" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="38.25">
       <c r="A7" t="s">
         <v>121</v>
       </c>
-      <c r="B7" t="s">
-        <v>165</v>
+      <c r="B7" s="5" t="s">
+        <v>164</v>
       </c>
       <c r="C7" t="s">
+        <v>200</v>
+      </c>
+      <c r="D7" t="s">
         <v>201</v>
       </c>
-      <c r="D7" t="s">
-        <v>150</v>
-      </c>
       <c r="E7">
+        <v>40</v>
+      </c>
+      <c r="F7">
+        <v>15</v>
+      </c>
+      <c r="G7">
         <v>30</v>
       </c>
-      <c r="F7">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9">
+      <c r="H7">
+        <v>25</v>
+      </c>
+      <c r="I7" s="7" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="25.5">
       <c r="A8" t="s">
         <v>122</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="5" t="s">
         <v>93</v>
       </c>
       <c r="C8" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D8" t="s">
-        <v>150</v>
+        <v>201</v>
       </c>
       <c r="E8">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="F8">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9">
+        <v>10</v>
+      </c>
+      <c r="G8">
+        <v>20</v>
+      </c>
+      <c r="H8">
+        <v>10</v>
+      </c>
+      <c r="I8" s="7" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="51">
       <c r="A9" t="s">
         <v>123</v>
       </c>
-      <c r="B9" t="s">
-        <v>151</v>
+      <c r="B9" s="1" t="s">
+        <v>150</v>
       </c>
       <c r="C9" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D9" t="s">
-        <v>150</v>
+        <v>201</v>
       </c>
       <c r="E9">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="F9">
-        <v>80</v>
+        <v>10</v>
+      </c>
+      <c r="G9">
+        <v>25</v>
+      </c>
+      <c r="H9">
+        <v>15</v>
+      </c>
+      <c r="I9" s="7" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="B13" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="B14" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="B15" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2">
+      <c r="B17" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2">
+      <c r="B18" t="s">
+        <v>228</v>
       </c>
     </row>
   </sheetData>
@@ -3781,15 +4134,15 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="28">
+    <row r="1" spans="1:9" ht="25.5">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -3816,6 +4169,118 @@
       </c>
       <c r="I1" s="10" t="s">
         <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" t="s">
+        <v>125</v>
+      </c>
+      <c r="B2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>171</v>
+      </c>
+      <c r="D2" s="17" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" t="s">
+        <v>126</v>
+      </c>
+      <c r="B3" t="s">
+        <v>79</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>171</v>
+      </c>
+      <c r="D3" s="17" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" t="s">
+        <v>127</v>
+      </c>
+      <c r="B4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C4" s="17" t="s">
+        <v>200</v>
+      </c>
+      <c r="D4" s="17" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" t="s">
+        <v>128</v>
+      </c>
+      <c r="B5" t="s">
+        <v>81</v>
+      </c>
+      <c r="C5" s="17" t="s">
+        <v>200</v>
+      </c>
+      <c r="D5" s="17" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" t="s">
+        <v>129</v>
+      </c>
+      <c r="B6" t="s">
+        <v>82</v>
+      </c>
+      <c r="C6" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="D6" s="17" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" t="s">
+        <v>130</v>
+      </c>
+      <c r="B7" t="s">
+        <v>85</v>
+      </c>
+      <c r="C7" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="D7" s="17" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" t="s">
+        <v>131</v>
+      </c>
+      <c r="B8" t="s">
+        <v>86</v>
+      </c>
+      <c r="C8" s="17" t="s">
+        <v>199</v>
+      </c>
+      <c r="D8" s="17" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" t="s">
+        <v>132</v>
+      </c>
+      <c r="B9" t="s">
+        <v>87</v>
+      </c>
+      <c r="C9" s="17" t="s">
+        <v>199</v>
+      </c>
+      <c r="D9" s="17" t="s">
+        <v>229</v>
       </c>
     </row>
   </sheetData>
@@ -3832,9 +4297,9 @@
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="28">
+    <row r="1" spans="1:9" ht="25.5">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -3873,17 +4338,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView topLeftCell="A21" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="C25" sqref="A18:C25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75"/>
   <cols>
-    <col min="2" max="2" width="28.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="49.5" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="4" customFormat="1" ht="14">
+    <row r="1" spans="1:3" s="4" customFormat="1">
       <c r="A1" s="4" t="s">
         <v>107</v>
       </c>
@@ -3894,18 +4359,18 @@
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="34">
+    <row r="2" spans="1:3" ht="31.5">
       <c r="A2" t="s">
         <v>108</v>
       </c>
       <c r="B2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C2" s="12" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="17">
+    <row r="3" spans="1:3" ht="15.75">
       <c r="A3" t="s">
         <v>109</v>
       </c>
@@ -3916,7 +4381,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="17">
+    <row r="4" spans="1:3" ht="15.75">
       <c r="A4" t="s">
         <v>110</v>
       </c>
@@ -3927,7 +4392,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="34">
+    <row r="5" spans="1:3" ht="31.5">
       <c r="A5" t="s">
         <v>111</v>
       </c>
@@ -3938,7 +4403,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="17">
+    <row r="6" spans="1:3" ht="15.75">
       <c r="A6" t="s">
         <v>112</v>
       </c>
@@ -3949,7 +4414,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="17">
+    <row r="7" spans="1:3" ht="15.75">
       <c r="A7" t="s">
         <v>113</v>
       </c>
@@ -3960,7 +4425,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="51">
+    <row r="8" spans="1:3" ht="47.25">
       <c r="A8" t="s">
         <v>114</v>
       </c>
@@ -3971,18 +4436,18 @@
         <v>68</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="34">
+    <row r="9" spans="1:3" ht="31.5">
       <c r="A9" t="s">
         <v>115</v>
       </c>
       <c r="B9" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="34">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="31.5">
       <c r="A10" t="s">
         <v>116</v>
       </c>
@@ -3993,7 +4458,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="34">
+    <row r="11" spans="1:3" ht="31.5">
       <c r="A11" t="s">
         <v>117</v>
       </c>
@@ -4001,10 +4466,10 @@
         <v>71</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="34">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="31.5">
       <c r="A12" t="s">
         <v>118</v>
       </c>
@@ -4015,7 +4480,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="51">
+    <row r="13" spans="1:3" ht="47.25">
       <c r="A13" t="s">
         <v>119</v>
       </c>
@@ -4026,7 +4491,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="68">
+    <row r="14" spans="1:3" ht="63">
       <c r="A14" t="s">
         <v>120</v>
       </c>
@@ -4034,21 +4499,21 @@
         <v>75</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="34">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="31.5">
       <c r="A15" t="s">
         <v>121</v>
       </c>
       <c r="B15" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="17">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="15.75">
       <c r="A16" t="s">
         <v>122</v>
       </c>
@@ -4059,7 +4524,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="34">
+    <row r="17" spans="1:3" ht="31.5">
       <c r="A17" t="s">
         <v>123</v>
       </c>
@@ -4070,7 +4535,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="17">
+    <row r="18" spans="1:3" ht="15.75">
       <c r="A18" t="s">
         <v>124</v>
       </c>
@@ -4081,7 +4546,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="17">
+    <row r="19" spans="1:3" ht="15.75">
       <c r="A19" t="s">
         <v>125</v>
       </c>
@@ -4092,7 +4557,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="17">
+    <row r="20" spans="1:3" ht="15.75">
       <c r="A20" t="s">
         <v>126</v>
       </c>
@@ -4103,7 +4568,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="34">
+    <row r="21" spans="1:3" ht="31.5">
       <c r="A21" t="s">
         <v>127</v>
       </c>
@@ -4114,7 +4579,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="34">
+    <row r="22" spans="1:3" ht="31.5">
       <c r="A22" t="s">
         <v>128</v>
       </c>
@@ -4125,7 +4590,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="34">
+    <row r="23" spans="1:3" ht="31.5">
       <c r="A23" t="s">
         <v>129</v>
       </c>
@@ -4136,7 +4601,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="34">
+    <row r="24" spans="1:3" ht="31.5">
       <c r="A24" t="s">
         <v>130</v>
       </c>
@@ -4147,7 +4612,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="51">
+    <row r="25" spans="1:3" ht="47.25">
       <c r="A25" t="s">
         <v>131</v>
       </c>
@@ -4158,7 +4623,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="34">
+    <row r="26" spans="1:3" ht="31.5">
       <c r="A26" t="s">
         <v>132</v>
       </c>
@@ -4169,7 +4634,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="136">
+    <row r="27" spans="1:3" ht="126">
       <c r="A27" t="s">
         <v>133</v>
       </c>
@@ -4177,10 +4642,10 @@
         <v>89</v>
       </c>
       <c r="C27" s="12" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" ht="17">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="15.75">
       <c r="A28" t="s">
         <v>134</v>
       </c>
@@ -4191,7 +4656,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="34">
+    <row r="29" spans="1:3" ht="31.5">
       <c r="A29" t="s">
         <v>135</v>
       </c>
@@ -4199,10 +4664,10 @@
         <v>91</v>
       </c>
       <c r="C29" s="12" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" ht="17">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="15.75">
       <c r="A30" t="s">
         <v>136</v>
       </c>
@@ -4213,7 +4678,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="17">
+    <row r="31" spans="1:3" ht="15.75">
       <c r="A31" t="s">
         <v>137</v>
       </c>
@@ -4224,7 +4689,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="34">
+    <row r="32" spans="1:3" ht="31.5">
       <c r="A32" t="s">
         <v>138</v>
       </c>
@@ -4235,7 +4700,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="17">
+    <row r="33" spans="1:3" ht="15.75">
       <c r="A33" t="s">
         <v>139</v>
       </c>
@@ -4246,7 +4711,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="34">
+    <row r="34" spans="1:3" ht="31.5">
       <c r="A34" t="s">
         <v>140</v>
       </c>
@@ -4257,7 +4722,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="51">
+    <row r="35" spans="1:3" ht="47.25">
       <c r="A35" t="s">
         <v>141</v>
       </c>
@@ -4268,7 +4733,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="34">
+    <row r="36" spans="1:3" ht="31.5">
       <c r="A36" t="s">
         <v>142</v>
       </c>
@@ -4279,7 +4744,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="34">
+    <row r="37" spans="1:3" ht="31.5">
       <c r="A37" t="s">
         <v>143</v>
       </c>
@@ -4290,7 +4755,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="34">
+    <row r="38" spans="1:3" ht="31.5">
       <c r="A38" t="s">
         <v>144</v>
       </c>
@@ -4301,7 +4766,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="34">
+    <row r="39" spans="1:3" ht="31.5">
       <c r="A39" t="s">
         <v>145</v>
       </c>
@@ -4312,7 +4777,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="34">
+    <row r="40" spans="1:3" ht="31.5">
       <c r="A40" t="s">
         <v>146</v>
       </c>
@@ -4323,7 +4788,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="34">
+    <row r="41" spans="1:3" ht="31.5">
       <c r="A41" t="s">
         <v>147</v>
       </c>
@@ -4334,7 +4799,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="34">
+    <row r="42" spans="1:3" ht="31.5">
       <c r="A42" t="s">
         <v>148</v>
       </c>
@@ -4345,7 +4810,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="34">
+    <row r="43" spans="1:3" ht="31.5">
       <c r="A43" t="s">
         <v>149</v>
       </c>

</xml_diff>

<commit_message>
fixed user stories order
</commit_message>
<xml_diff>
--- a/TeamVOXSReport.xlsx
+++ b/TeamVOXSReport.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MS SE\SSW-555\Sanjeev Branch\SSW-555\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1FC6FAD-78FB-40E8-864F-C0396291EDEA}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53B429B7-AC3F-425F-9FA2-C75353126940}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="25605" windowHeight="14565" tabRatio="500" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="25605" windowHeight="14565" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -2127,15 +2127,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView topLeftCell="A36" zoomScale="150" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:B37"/>
+    <sheetView topLeftCell="A18" zoomScale="150" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="8.875" customWidth="1"/>
     <col min="2" max="2" width="23.5" customWidth="1"/>
-    <col min="3" max="3" width="52.875" customWidth="1"/>
+    <col min="3" max="3" width="67.625" customWidth="1"/>
     <col min="4" max="4" width="24.875" customWidth="1"/>
     <col min="5" max="5" width="20.875" customWidth="1"/>
     <col min="6" max="6" width="26.875" customWidth="1"/>
@@ -2662,7 +2662,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="31.5">
+    <row r="33" spans="1:4" ht="15.75">
       <c r="A33" t="s">
         <v>128</v>
       </c>
@@ -2676,7 +2676,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="31.5">
+    <row r="34" spans="1:4" ht="15.75">
       <c r="A34" t="s">
         <v>129</v>
       </c>
@@ -2690,7 +2690,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="31.5">
+    <row r="35" spans="1:4" ht="15.75">
       <c r="A35" t="s">
         <v>130</v>
       </c>
@@ -2718,7 +2718,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="47.25">
+    <row r="37" spans="1:4" ht="31.5">
       <c r="A37" t="s">
         <v>132</v>
       </c>
@@ -2752,8 +2752,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="150" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19:E26"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10:C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75"/>
@@ -3413,7 +3413,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+    <sheetView zoomScale="150" workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -3833,13 +3833,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:I18"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="150" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView zoomScale="150" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75"/>
+  <cols>
+    <col min="2" max="2" width="25.875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="25.5">
+    <row r="1" spans="1:9">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -3873,7 +3876,7 @@
         <v>116</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>203</v>
+        <v>76</v>
       </c>
       <c r="C2" s="17" t="s">
         <v>171</v>
@@ -3897,12 +3900,12 @@
         <v>202</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="38.25">
+    <row r="3" spans="1:9">
       <c r="A3" t="s">
         <v>117</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>204</v>
+      <c r="B3" t="s">
+        <v>203</v>
       </c>
       <c r="C3" t="s">
         <v>171</v>
@@ -3926,12 +3929,12 @@
         <v>202</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="38.25">
+    <row r="4" spans="1:9">
       <c r="A4" t="s">
         <v>118</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>205</v>
+      <c r="B4" t="s">
+        <v>204</v>
       </c>
       <c r="C4" t="s">
         <v>175</v>
@@ -3955,12 +3958,12 @@
         <v>202</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="25.5">
+    <row r="5" spans="1:9">
       <c r="A5" t="s">
         <v>119</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>73</v>
+      <c r="B5" t="s">
+        <v>205</v>
       </c>
       <c r="C5" t="s">
         <v>175</v>
@@ -3984,12 +3987,12 @@
         <v>202</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="25.5">
+    <row r="6" spans="1:9">
       <c r="A6" t="s">
         <v>120</v>
       </c>
-      <c r="B6" s="5" t="s">
-        <v>206</v>
+      <c r="B6" t="s">
+        <v>63</v>
       </c>
       <c r="C6" t="s">
         <v>200</v>
@@ -4013,12 +4016,12 @@
         <v>202</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="38.25">
+    <row r="7" spans="1:9">
       <c r="A7" t="s">
         <v>121</v>
       </c>
-      <c r="B7" s="5" t="s">
-        <v>164</v>
+      <c r="B7" t="s">
+        <v>206</v>
       </c>
       <c r="C7" t="s">
         <v>200</v>
@@ -4042,12 +4045,12 @@
         <v>202</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="25.5">
+    <row r="8" spans="1:9">
       <c r="A8" t="s">
         <v>122</v>
       </c>
-      <c r="B8" s="5" t="s">
-        <v>93</v>
+      <c r="B8" t="s">
+        <v>164</v>
       </c>
       <c r="C8" t="s">
         <v>199</v>
@@ -4071,12 +4074,12 @@
         <v>202</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="51">
+    <row r="9" spans="1:9">
       <c r="A9" t="s">
         <v>123</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>150</v>
+      <c r="B9" t="s">
+        <v>93</v>
       </c>
       <c r="C9" t="s">
         <v>199</v>

</xml_diff>

<commit_message>
Added sprint 3 user stories
</commit_message>
<xml_diff>
--- a/TeamVOXSReport.xlsx
+++ b/TeamVOXSReport.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MS SE\SSW-555\Sanjeev Branch\SSW-555\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53B429B7-AC3F-425F-9FA2-C75353126940}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{481D75C7-BCB6-45BB-8F25-482435A1555B}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="25605" windowHeight="14565" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="25605" windowHeight="14565" tabRatio="794" firstSheet="1" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="557" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="553" uniqueCount="230">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -2752,15 +2752,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10:C18"/>
+    <sheetView topLeftCell="A7" zoomScale="150" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="5.125" customWidth="1"/>
     <col min="2" max="2" width="7.625" customWidth="1"/>
-    <col min="3" max="3" width="24.125" customWidth="1"/>
+    <col min="3" max="3" width="30.5" customWidth="1"/>
     <col min="4" max="4" width="9.125" customWidth="1"/>
     <col min="5" max="5" width="7.625" customWidth="1"/>
   </cols>
@@ -2790,10 +2790,10 @@
         <v>108</v>
       </c>
       <c r="C2" t="s">
-        <v>82</v>
+        <v>150</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>175</v>
+        <v>199</v>
       </c>
       <c r="E2" t="s">
         <v>201</v>
@@ -2807,10 +2807,10 @@
         <v>109</v>
       </c>
       <c r="C3" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D3" s="17" t="s">
-        <v>171</v>
+        <v>200</v>
       </c>
       <c r="E3" t="s">
         <v>201</v>
@@ -2824,7 +2824,7 @@
         <v>110</v>
       </c>
       <c r="C4" t="s">
-        <v>77</v>
+        <v>62</v>
       </c>
       <c r="D4" s="17" t="s">
         <v>199</v>
@@ -2841,7 +2841,7 @@
         <v>111</v>
       </c>
       <c r="C5" t="s">
-        <v>94</v>
+        <v>64</v>
       </c>
       <c r="D5" s="17" t="s">
         <v>199</v>
@@ -2858,7 +2858,7 @@
         <v>112</v>
       </c>
       <c r="C6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D6" s="17" t="s">
         <v>175</v>
@@ -2874,8 +2874,8 @@
       <c r="B7" t="s">
         <v>113</v>
       </c>
-      <c r="C7" s="17" t="s">
-        <v>71</v>
+      <c r="C7" t="s">
+        <v>66</v>
       </c>
       <c r="D7" s="17" t="s">
         <v>171</v>
@@ -2891,8 +2891,8 @@
       <c r="B8" t="s">
         <v>114</v>
       </c>
-      <c r="C8" s="17" t="s">
-        <v>79</v>
+      <c r="C8" t="s">
+        <v>67</v>
       </c>
       <c r="D8" s="17" t="s">
         <v>171</v>
@@ -2908,8 +2908,8 @@
       <c r="B9" t="s">
         <v>115</v>
       </c>
-      <c r="C9" s="17" t="s">
-        <v>85</v>
+      <c r="C9" t="s">
+        <v>151</v>
       </c>
       <c r="D9" s="17" t="s">
         <v>175</v>
@@ -2922,11 +2922,11 @@
       <c r="A10">
         <v>2</v>
       </c>
-      <c r="B10" s="17" t="s">
+      <c r="B10" t="s">
         <v>116</v>
       </c>
-      <c r="C10" s="17" t="s">
-        <v>76</v>
+      <c r="C10" t="s">
+        <v>69</v>
       </c>
       <c r="D10" s="17" t="s">
         <v>199</v>
@@ -2943,7 +2943,7 @@
         <v>117</v>
       </c>
       <c r="C11" t="s">
-        <v>203</v>
+        <v>71</v>
       </c>
       <c r="D11" s="17" t="s">
         <v>171</v>
@@ -2960,7 +2960,7 @@
         <v>118</v>
       </c>
       <c r="C12" t="s">
-        <v>204</v>
+        <v>72</v>
       </c>
       <c r="D12" s="17" t="s">
         <v>171</v>
@@ -2977,7 +2977,7 @@
         <v>119</v>
       </c>
       <c r="C13" t="s">
-        <v>205</v>
+        <v>73</v>
       </c>
       <c r="D13" s="17" t="s">
         <v>200</v>
@@ -2994,7 +2994,7 @@
         <v>120</v>
       </c>
       <c r="C14" t="s">
-        <v>63</v>
+        <v>75</v>
       </c>
       <c r="D14" s="17" t="s">
         <v>200</v>
@@ -3011,7 +3011,7 @@
         <v>121</v>
       </c>
       <c r="C15" t="s">
-        <v>206</v>
+        <v>164</v>
       </c>
       <c r="D15" s="17" t="s">
         <v>175</v>
@@ -3028,7 +3028,7 @@
         <v>122</v>
       </c>
       <c r="C16" t="s">
-        <v>164</v>
+        <v>76</v>
       </c>
       <c r="D16" s="17" t="s">
         <v>175</v>
@@ -3045,7 +3045,7 @@
         <v>123</v>
       </c>
       <c r="C17" t="s">
-        <v>93</v>
+        <v>77</v>
       </c>
       <c r="D17" s="17" t="s">
         <v>199</v>
@@ -3056,13 +3056,13 @@
     </row>
     <row r="18" spans="1:5">
       <c r="A18">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B18" t="s">
         <v>124</v>
       </c>
       <c r="C18" t="s">
-        <v>150</v>
+        <v>78</v>
       </c>
       <c r="D18" s="17" t="s">
         <v>199</v>
@@ -3079,13 +3079,13 @@
         <v>125</v>
       </c>
       <c r="C19" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D19" s="17" t="s">
         <v>171</v>
       </c>
       <c r="E19" s="17" t="s">
-        <v>229</v>
+        <v>201</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -3096,13 +3096,13 @@
         <v>126</v>
       </c>
       <c r="C20" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D20" s="17" t="s">
         <v>171</v>
       </c>
       <c r="E20" s="17" t="s">
-        <v>229</v>
+        <v>201</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -3113,13 +3113,13 @@
         <v>127</v>
       </c>
       <c r="C21" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D21" s="17" t="s">
         <v>200</v>
       </c>
       <c r="E21" s="17" t="s">
-        <v>229</v>
+        <v>201</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -3130,13 +3130,13 @@
         <v>128</v>
       </c>
       <c r="C22" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D22" s="17" t="s">
         <v>200</v>
       </c>
       <c r="E22" s="17" t="s">
-        <v>229</v>
+        <v>201</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -3147,13 +3147,13 @@
         <v>129</v>
       </c>
       <c r="C23" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="D23" s="17" t="s">
         <v>175</v>
       </c>
       <c r="E23" s="17" t="s">
-        <v>229</v>
+        <v>201</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -3164,13 +3164,13 @@
         <v>130</v>
       </c>
       <c r="C24" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D24" s="17" t="s">
         <v>175</v>
       </c>
       <c r="E24" s="17" t="s">
-        <v>229</v>
+        <v>201</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -3181,31 +3181,18 @@
         <v>131</v>
       </c>
       <c r="C25" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D25" s="17" t="s">
         <v>199</v>
       </c>
       <c r="E25" s="17" t="s">
-        <v>229</v>
+        <v>201</v>
       </c>
     </row>
     <row r="26" spans="1:5">
-      <c r="A26">
-        <v>3</v>
-      </c>
-      <c r="B26" t="s">
-        <v>132</v>
-      </c>
-      <c r="C26" t="s">
-        <v>87</v>
-      </c>
-      <c r="D26" s="17" t="s">
-        <v>199</v>
-      </c>
-      <c r="E26" s="17" t="s">
-        <v>229</v>
-      </c>
+      <c r="D26" s="17"/>
+      <c r="E26" s="17"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -3515,8 +3502,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:I18"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="150" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView zoomScale="150" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75"/>
@@ -3565,7 +3552,7 @@
         <v>108</v>
       </c>
       <c r="B2" t="s">
-        <v>82</v>
+        <v>150</v>
       </c>
       <c r="C2" s="17" t="s">
         <v>175</v>
@@ -3594,7 +3581,7 @@
         <v>109</v>
       </c>
       <c r="B3" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C3" s="17" t="s">
         <v>171</v>
@@ -3623,7 +3610,7 @@
         <v>110</v>
       </c>
       <c r="B4" t="s">
-        <v>77</v>
+        <v>62</v>
       </c>
       <c r="C4" s="17" t="s">
         <v>199</v>
@@ -3652,7 +3639,7 @@
         <v>111</v>
       </c>
       <c r="B5" t="s">
-        <v>94</v>
+        <v>64</v>
       </c>
       <c r="C5" s="17" t="s">
         <v>199</v>
@@ -3681,7 +3668,7 @@
         <v>112</v>
       </c>
       <c r="B6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C6" s="17" t="s">
         <v>175</v>
@@ -3709,8 +3696,8 @@
       <c r="A7" t="s">
         <v>113</v>
       </c>
-      <c r="B7" s="17" t="s">
-        <v>71</v>
+      <c r="B7" t="s">
+        <v>66</v>
       </c>
       <c r="C7" s="17" t="s">
         <v>200</v>
@@ -3738,8 +3725,8 @@
       <c r="A8" t="s">
         <v>114</v>
       </c>
-      <c r="B8" s="17" t="s">
-        <v>79</v>
+      <c r="B8" t="s">
+        <v>67</v>
       </c>
       <c r="C8" s="17" t="s">
         <v>171</v>
@@ -3767,8 +3754,8 @@
       <c r="A9" t="s">
         <v>115</v>
       </c>
-      <c r="B9" s="17" t="s">
-        <v>85</v>
+      <c r="B9" t="s">
+        <v>151</v>
       </c>
       <c r="C9" s="17" t="s">
         <v>200</v>
@@ -3834,7 +3821,7 @@
   <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="A2" sqref="A2:B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75"/>
@@ -3872,11 +3859,11 @@
       </c>
     </row>
     <row r="2" spans="1:9">
-      <c r="A2" s="17" t="s">
+      <c r="A2" t="s">
         <v>116</v>
       </c>
-      <c r="B2" s="17" t="s">
-        <v>76</v>
+      <c r="B2" t="s">
+        <v>69</v>
       </c>
       <c r="C2" s="17" t="s">
         <v>171</v>
@@ -3905,7 +3892,7 @@
         <v>117</v>
       </c>
       <c r="B3" t="s">
-        <v>203</v>
+        <v>71</v>
       </c>
       <c r="C3" t="s">
         <v>171</v>
@@ -3934,7 +3921,7 @@
         <v>118</v>
       </c>
       <c r="B4" t="s">
-        <v>204</v>
+        <v>72</v>
       </c>
       <c r="C4" t="s">
         <v>175</v>
@@ -3963,7 +3950,7 @@
         <v>119</v>
       </c>
       <c r="B5" t="s">
-        <v>205</v>
+        <v>73</v>
       </c>
       <c r="C5" t="s">
         <v>175</v>
@@ -3992,7 +3979,7 @@
         <v>120</v>
       </c>
       <c r="B6" t="s">
-        <v>63</v>
+        <v>75</v>
       </c>
       <c r="C6" t="s">
         <v>200</v>
@@ -4021,7 +4008,7 @@
         <v>121</v>
       </c>
       <c r="B7" t="s">
-        <v>206</v>
+        <v>164</v>
       </c>
       <c r="C7" t="s">
         <v>200</v>
@@ -4050,7 +4037,7 @@
         <v>122</v>
       </c>
       <c r="B8" t="s">
-        <v>164</v>
+        <v>76</v>
       </c>
       <c r="C8" t="s">
         <v>199</v>
@@ -4079,7 +4066,7 @@
         <v>123</v>
       </c>
       <c r="B9" t="s">
-        <v>93</v>
+        <v>77</v>
       </c>
       <c r="C9" t="s">
         <v>199</v>
@@ -4140,10 +4127,13 @@
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75"/>
+  <cols>
+    <col min="2" max="2" width="28.375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="25.5">
       <c r="A1" s="4" t="s">
@@ -4176,7 +4166,7 @@
     </row>
     <row r="2" spans="1:9">
       <c r="A2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B2" t="s">
         <v>78</v>
@@ -4190,7 +4180,7 @@
     </row>
     <row r="3" spans="1:9">
       <c r="A3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B3" t="s">
         <v>79</v>
@@ -4204,7 +4194,7 @@
     </row>
     <row r="4" spans="1:9">
       <c r="A4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B4" t="s">
         <v>80</v>
@@ -4218,7 +4208,7 @@
     </row>
     <row r="5" spans="1:9">
       <c r="A5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B5" t="s">
         <v>81</v>
@@ -4232,7 +4222,7 @@
     </row>
     <row r="6" spans="1:9">
       <c r="A6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B6" t="s">
         <v>82</v>
@@ -4246,7 +4236,7 @@
     </row>
     <row r="7" spans="1:9">
       <c r="A7" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B7" t="s">
         <v>85</v>
@@ -4260,7 +4250,7 @@
     </row>
     <row r="8" spans="1:9">
       <c r="A8" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B8" t="s">
         <v>86</v>
@@ -4274,7 +4264,7 @@
     </row>
     <row r="9" spans="1:9">
       <c r="A9" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B9" t="s">
         <v>87</v>
@@ -4341,8 +4331,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="C25" sqref="A18:C25"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75"/>

</xml_diff>

<commit_message>
Added all user stories
</commit_message>
<xml_diff>
--- a/TeamVOXSReport.xlsx
+++ b/TeamVOXSReport.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21001"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MS SE\SSW-555\Sanjeev Branch\SSW-555\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{514C9721-5FF4-4377-B240-C4935592FC67}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{280A6237-A57D-4F4E-BA66-D89BA15D640B}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="25605" windowHeight="14565" tabRatio="794" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="25605" windowHeight="14565" tabRatio="794" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="593" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="648" uniqueCount="214">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -617,30 +617,6 @@
   </si>
   <si>
     <t>Estimated Size</t>
-  </si>
-  <si>
-    <t>Husband should be a male and Wife should be a female</t>
-  </si>
-  <si>
-    <t>Divorce can only occur before death</t>
-  </si>
-  <si>
-    <t>The last name of all male members should be same</t>
-  </si>
-  <si>
-    <t>Age shouldn't be above 150</t>
-  </si>
-  <si>
-    <t>List all people who are above 30 and alive yet not married.</t>
-  </si>
-  <si>
-    <t>No one should be married before 14</t>
-  </si>
-  <si>
-    <t>siblings shouldn't marry each other</t>
-  </si>
-  <si>
-    <t>All individual and family ids should be unique</t>
   </si>
   <si>
     <r>
@@ -662,9 +638,6 @@
     </r>
   </si>
   <si>
-    <t>Maximum 15 siblings in a family</t>
-  </si>
-  <si>
     <t>Status</t>
   </si>
   <si>
@@ -690,30 +663,6 @@
   </si>
   <si>
     <t>Yes</t>
-  </si>
-  <si>
-    <t>Marriage Before Death</t>
-  </si>
-  <si>
-    <t>Unique First name Families</t>
-  </si>
-  <si>
-    <t>Marriage before Divorced</t>
-  </si>
-  <si>
-    <t>Sibling Spacing</t>
-  </si>
-  <si>
-    <t>Check if Marriage date is before Death date</t>
-  </si>
-  <si>
-    <t>Check if all first names in families are unique</t>
-  </si>
-  <si>
-    <t>Birth date of an individual should occur before marriage date</t>
-  </si>
-  <si>
-    <t>Marriage date of an indivdual should occur before divorce date</t>
   </si>
   <si>
     <t>Things to do:</t>
@@ -758,18 +707,10 @@
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
-    <t>Birth dates of siblings should be more than 8 months apart or less than 2 days apart (twins may be born one day apart, e.g. 11:59 PM and 12:02 AM the following calendar day)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>No more than five siblings should be born at the same time</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
-    <t>No more than five siblings should be born at the same time</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>Use Github Better</t>
   </si>
   <si>
@@ -786,6 +727,9 @@
   </si>
   <si>
     <t>List Living single</t>
+  </si>
+  <si>
+    <t>List upcoming Birthdays</t>
   </si>
 </sst>
 </file>
@@ -1227,6 +1171,9 @@
                 <c:pt idx="2">
                   <c:v>41927</c:v>
                 </c:pt>
+                <c:pt idx="3">
+                  <c:v>41957</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -1244,6 +1191,9 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2131,10 +2081,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G37"/>
+  <dimension ref="A1:G44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="150" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView topLeftCell="A38" zoomScale="150" workbookViewId="0">
+      <selection activeCell="A40" sqref="A40:B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75"/>
@@ -2156,7 +2106,7 @@
         <v>20</v>
       </c>
       <c r="C1" s="18" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>21</v>
@@ -2201,7 +2151,7 @@
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="17" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
       <c r="B5" t="s">
         <v>179</v>
@@ -2213,29 +2163,29 @@
         <v>181</v>
       </c>
       <c r="E5" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="17" t="s">
-        <v>217</v>
+        <v>200</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>218</v>
+        <v>201</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>219</v>
+        <v>202</v>
       </c>
       <c r="D6" s="16" t="s">
-        <v>220</v>
+        <v>203</v>
       </c>
       <c r="E6" s="17" t="s">
-        <v>221</v>
+        <v>204</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="C7" s="17" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -2259,21 +2209,21 @@
         <v>183</v>
       </c>
       <c r="F11" s="18" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
       <c r="G11" s="18" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="31.5">
       <c r="A13" t="s">
         <v>108</v>
       </c>
       <c r="B13" t="s">
-        <v>82</v>
-      </c>
-      <c r="C13" s="17" t="s">
-        <v>184</v>
+        <v>150</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>30</v>
       </c>
       <c r="D13" s="17" t="s">
         <v>175</v>
@@ -2285,18 +2235,18 @@
         <v>130</v>
       </c>
       <c r="G13" s="17" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="15.75">
       <c r="A14" t="s">
         <v>109</v>
       </c>
       <c r="B14" t="s">
-        <v>66</v>
-      </c>
-      <c r="C14" s="17" t="s">
-        <v>185</v>
+        <v>63</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>31</v>
       </c>
       <c r="D14" s="17" t="s">
         <v>171</v>
@@ -2308,21 +2258,21 @@
         <v>100</v>
       </c>
       <c r="G14" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="15.75">
       <c r="A15" t="s">
         <v>110</v>
       </c>
       <c r="B15" t="s">
-        <v>77</v>
-      </c>
-      <c r="C15" s="17" t="s">
-        <v>186</v>
+        <v>62</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>32</v>
       </c>
       <c r="D15" s="17" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
       <c r="E15">
         <v>110</v>
@@ -2331,21 +2281,21 @@
         <v>150</v>
       </c>
       <c r="G15" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="31.5">
       <c r="A16" t="s">
         <v>111</v>
       </c>
       <c r="B16" t="s">
-        <v>94</v>
-      </c>
-      <c r="C16" s="17" t="s">
-        <v>188</v>
+        <v>64</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>33</v>
       </c>
       <c r="D16" s="17" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
       <c r="E16">
         <v>140</v>
@@ -2354,18 +2304,18 @@
         <v>180</v>
       </c>
       <c r="G16" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="15.75">
       <c r="A17" t="s">
         <v>112</v>
       </c>
       <c r="B17" t="s">
-        <v>67</v>
-      </c>
-      <c r="C17" s="17" t="s">
-        <v>187</v>
+        <v>65</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>34</v>
       </c>
       <c r="D17" s="17" t="s">
         <v>175</v>
@@ -2377,18 +2327,18 @@
         <v>100</v>
       </c>
       <c r="G17" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="15.75">
       <c r="A18" t="s">
         <v>113</v>
       </c>
-      <c r="B18" s="17" t="s">
-        <v>71</v>
-      </c>
-      <c r="C18" s="17" t="s">
-        <v>189</v>
+      <c r="B18" t="s">
+        <v>66</v>
+      </c>
+      <c r="C18" s="12" t="s">
+        <v>35</v>
       </c>
       <c r="D18" s="17" t="s">
         <v>171</v>
@@ -2400,18 +2350,18 @@
         <v>105</v>
       </c>
       <c r="G18" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="31.5">
       <c r="A19" t="s">
         <v>114</v>
       </c>
-      <c r="B19" s="17" t="s">
-        <v>79</v>
-      </c>
-      <c r="C19" s="17" t="s">
-        <v>190</v>
+      <c r="B19" t="s">
+        <v>67</v>
+      </c>
+      <c r="C19" s="12" t="s">
+        <v>68</v>
       </c>
       <c r="D19" s="17" t="s">
         <v>171</v>
@@ -2423,18 +2373,18 @@
         <v>120</v>
       </c>
       <c r="G19" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="31.5">
       <c r="A20" t="s">
         <v>115</v>
       </c>
-      <c r="B20" s="17" t="s">
-        <v>85</v>
-      </c>
-      <c r="C20" s="17" t="s">
-        <v>191</v>
+      <c r="B20" t="s">
+        <v>151</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>165</v>
       </c>
       <c r="D20" s="17" t="s">
         <v>175</v>
@@ -2446,21 +2396,21 @@
         <v>110</v>
       </c>
       <c r="G20" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7">
-      <c r="A21" s="17" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="31.5">
+      <c r="A21" t="s">
         <v>116</v>
       </c>
-      <c r="B21" s="17" t="s">
-        <v>76</v>
-      </c>
-      <c r="C21" s="17" t="s">
-        <v>193</v>
+      <c r="B21" t="s">
+        <v>69</v>
+      </c>
+      <c r="C21" s="12" t="s">
+        <v>70</v>
       </c>
       <c r="D21" s="17" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
       <c r="E21">
         <v>80</v>
@@ -2469,18 +2419,18 @@
         <v>120</v>
       </c>
       <c r="G21" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="31.5">
       <c r="A22" t="s">
         <v>117</v>
       </c>
       <c r="B22" t="s">
-        <v>203</v>
-      </c>
-      <c r="C22" s="17" t="s">
-        <v>207</v>
+        <v>71</v>
+      </c>
+      <c r="C22" s="12" t="s">
+        <v>166</v>
       </c>
       <c r="D22" t="s">
         <v>171</v>
@@ -2492,15 +2442,15 @@
         <v>80</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:7" ht="15.75">
       <c r="A23" t="s">
         <v>118</v>
       </c>
       <c r="B23" t="s">
-        <v>204</v>
-      </c>
-      <c r="C23" s="17" t="s">
-        <v>208</v>
+        <v>72</v>
+      </c>
+      <c r="C23" s="12" t="s">
+        <v>36</v>
       </c>
       <c r="D23" t="s">
         <v>171</v>
@@ -2512,15 +2462,15 @@
         <v>80</v>
       </c>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:7" ht="31.5">
       <c r="A24" t="s">
         <v>119</v>
       </c>
       <c r="B24" t="s">
-        <v>205</v>
-      </c>
-      <c r="C24" s="17" t="s">
-        <v>210</v>
+        <v>73</v>
+      </c>
+      <c r="C24" s="12" t="s">
+        <v>74</v>
       </c>
       <c r="D24" t="s">
         <v>175</v>
@@ -2532,15 +2482,15 @@
         <v>80</v>
       </c>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:7" ht="47.25">
       <c r="A25" t="s">
         <v>120</v>
       </c>
       <c r="B25" t="s">
-        <v>63</v>
-      </c>
-      <c r="C25" t="s">
-        <v>209</v>
+        <v>75</v>
+      </c>
+      <c r="C25" s="12" t="s">
+        <v>205</v>
       </c>
       <c r="D25" t="s">
         <v>175</v>
@@ -2552,18 +2502,18 @@
         <v>80</v>
       </c>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:7" ht="15.75">
       <c r="A26" t="s">
         <v>121</v>
       </c>
       <c r="B26" t="s">
+        <v>164</v>
+      </c>
+      <c r="C26" s="12" t="s">
         <v>206</v>
       </c>
-      <c r="C26" s="17" t="s">
-        <v>223</v>
-      </c>
       <c r="D26" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="E26">
         <v>30</v>
@@ -2572,18 +2522,18 @@
         <v>80</v>
       </c>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:7" ht="15.75">
       <c r="A27" t="s">
         <v>122</v>
       </c>
       <c r="B27" t="s">
-        <v>164</v>
-      </c>
-      <c r="C27" s="17" t="s">
-        <v>225</v>
+        <v>76</v>
+      </c>
+      <c r="C27" s="12" t="s">
+        <v>37</v>
       </c>
       <c r="D27" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="E27">
         <v>30</v>
@@ -2592,15 +2542,18 @@
         <v>80</v>
       </c>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:7" ht="15.75">
       <c r="A28" t="s">
         <v>123</v>
       </c>
       <c r="B28" t="s">
-        <v>93</v>
+        <v>77</v>
+      </c>
+      <c r="C28" s="12" t="s">
+        <v>38</v>
       </c>
       <c r="D28" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
       <c r="E28">
         <v>30</v>
@@ -2609,15 +2562,18 @@
         <v>80</v>
       </c>
     </row>
-    <row r="29" spans="1:7">
+    <row r="29" spans="1:7" ht="15.75">
       <c r="A29" t="s">
         <v>124</v>
       </c>
       <c r="B29" t="s">
-        <v>150</v>
+        <v>78</v>
+      </c>
+      <c r="C29" s="12" t="s">
+        <v>39</v>
       </c>
       <c r="D29" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
       <c r="E29">
         <v>30</v>
@@ -2631,10 +2587,10 @@
         <v>125</v>
       </c>
       <c r="B30" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C30" s="12" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D30" t="s">
         <v>171</v>
@@ -2642,13 +2598,13 @@
     </row>
     <row r="31" spans="1:7" ht="15.75">
       <c r="A31" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B31" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="C31" s="12" t="s">
-        <v>40</v>
+        <v>83</v>
       </c>
       <c r="D31" t="s">
         <v>171</v>
@@ -2656,41 +2612,41 @@
     </row>
     <row r="32" spans="1:7" ht="15.75">
       <c r="A32" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B32" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="C32" s="12" t="s">
-        <v>41</v>
+        <v>84</v>
       </c>
       <c r="D32" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" ht="15.75">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="31.5">
       <c r="A33" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B33" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="C33" s="12" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D33" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" ht="15.75">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="31.5">
       <c r="A34" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="B34" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="C34" s="12" t="s">
-        <v>83</v>
+        <v>45</v>
       </c>
       <c r="D34" t="s">
         <v>175</v>
@@ -2698,13 +2654,13 @@
     </row>
     <row r="35" spans="1:4" ht="15.75">
       <c r="A35" t="s">
-        <v>130</v>
+        <v>137</v>
       </c>
       <c r="B35" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="C35" s="12" t="s">
-        <v>84</v>
+        <v>48</v>
       </c>
       <c r="D35" t="s">
         <v>175</v>
@@ -2712,30 +2668,107 @@
     </row>
     <row r="36" spans="1:4" ht="31.5">
       <c r="A36" t="s">
+        <v>138</v>
+      </c>
+      <c r="B36" t="s">
+        <v>94</v>
+      </c>
+      <c r="C36" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="D36" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="15.75">
+      <c r="A37" t="s">
+        <v>126</v>
+      </c>
+      <c r="B37" t="s">
+        <v>80</v>
+      </c>
+      <c r="C37" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="D37" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="15.75">
+      <c r="A38" t="s">
+        <v>127</v>
+      </c>
+      <c r="B38" t="s">
+        <v>81</v>
+      </c>
+      <c r="C38" s="12" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="31.5">
+      <c r="A39" t="s">
         <v>131</v>
       </c>
-      <c r="B36" t="s">
-        <v>86</v>
-      </c>
-      <c r="C36" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="D36" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" ht="31.5">
-      <c r="A37" t="s">
-        <v>132</v>
-      </c>
-      <c r="B37" t="s">
+      <c r="B39" t="s">
         <v>87</v>
       </c>
-      <c r="C37" s="12" t="s">
+      <c r="C39" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="D37" t="s">
-        <v>199</v>
+    </row>
+    <row r="40" spans="1:4" ht="31.5">
+      <c r="A40" t="s">
+        <v>145</v>
+      </c>
+      <c r="B40" t="s">
+        <v>213</v>
+      </c>
+      <c r="C40" s="12" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="15.75">
+      <c r="A41" t="s">
+        <v>135</v>
+      </c>
+      <c r="B41" t="s">
+        <v>91</v>
+      </c>
+      <c r="C41" s="12" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="15.75">
+      <c r="A42" t="s">
+        <v>139</v>
+      </c>
+      <c r="B42" t="s">
+        <v>95</v>
+      </c>
+      <c r="C42" s="12" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="31.5">
+      <c r="A43" t="s">
+        <v>140</v>
+      </c>
+      <c r="B43" t="s">
+        <v>96</v>
+      </c>
+      <c r="C43" s="12" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="31.5">
+      <c r="A44" t="s">
+        <v>141</v>
+      </c>
+      <c r="B44" t="s">
+        <v>106</v>
+      </c>
+      <c r="C44" s="12" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -2756,10 +2789,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="150" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView topLeftCell="A19" zoomScale="150" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29:C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75"/>
@@ -2799,10 +2832,10 @@
         <v>150</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
       <c r="E2" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -2816,10 +2849,10 @@
         <v>63</v>
       </c>
       <c r="D3" s="17" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="E3" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -2833,10 +2866,10 @@
         <v>62</v>
       </c>
       <c r="D4" s="17" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
       <c r="E4" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -2850,10 +2883,10 @@
         <v>64</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
       <c r="E5" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -2870,7 +2903,7 @@
         <v>175</v>
       </c>
       <c r="E6" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -2887,7 +2920,7 @@
         <v>171</v>
       </c>
       <c r="E7" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -2904,7 +2937,7 @@
         <v>171</v>
       </c>
       <c r="E8" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -2921,7 +2954,7 @@
         <v>175</v>
       </c>
       <c r="E9" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -2935,10 +2968,10 @@
         <v>69</v>
       </c>
       <c r="D10" s="17" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
       <c r="E10" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -2955,7 +2988,7 @@
         <v>171</v>
       </c>
       <c r="E11" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -2972,7 +3005,7 @@
         <v>171</v>
       </c>
       <c r="E12" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -2986,10 +3019,10 @@
         <v>73</v>
       </c>
       <c r="D13" s="17" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="E13" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -3003,10 +3036,10 @@
         <v>75</v>
       </c>
       <c r="D14" s="17" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="E14" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -3023,7 +3056,7 @@
         <v>175</v>
       </c>
       <c r="E15" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -3040,7 +3073,7 @@
         <v>175</v>
       </c>
       <c r="E16" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -3054,10 +3087,10 @@
         <v>77</v>
       </c>
       <c r="D17" s="17" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
       <c r="E17" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -3074,7 +3107,7 @@
         <v>171</v>
       </c>
       <c r="E18" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -3091,7 +3124,7 @@
         <v>171</v>
       </c>
       <c r="E19" s="17" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -3099,16 +3132,16 @@
         <v>3</v>
       </c>
       <c r="B20" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="C20" t="s">
-        <v>230</v>
+        <v>82</v>
       </c>
       <c r="D20" s="17" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="E20" s="17" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -3116,16 +3149,16 @@
         <v>3</v>
       </c>
       <c r="B21" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
       <c r="C21" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="D21" s="17" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="E21" s="17" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -3133,16 +3166,16 @@
         <v>3</v>
       </c>
       <c r="B22" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="C22" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="D22" s="17" t="s">
         <v>175</v>
       </c>
       <c r="E22" s="17" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -3150,16 +3183,16 @@
         <v>3</v>
       </c>
       <c r="B23" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="C23" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="D23" s="17" t="s">
         <v>175</v>
       </c>
       <c r="E23" s="17" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -3167,16 +3200,16 @@
         <v>3</v>
       </c>
       <c r="B24" t="s">
-        <v>130</v>
+        <v>137</v>
       </c>
       <c r="C24" t="s">
-        <v>86</v>
+        <v>93</v>
       </c>
       <c r="D24" s="17" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
       <c r="E24" s="17" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -3184,21 +3217,153 @@
         <v>3</v>
       </c>
       <c r="B25" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C25" t="s">
-        <v>231</v>
+        <v>94</v>
       </c>
       <c r="D25" s="17" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
       <c r="E25" s="17" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
     </row>
     <row r="26" spans="1:5">
-      <c r="D26" s="17"/>
-      <c r="E26" s="17"/>
+      <c r="A26">
+        <v>4</v>
+      </c>
+      <c r="B26" t="s">
+        <v>126</v>
+      </c>
+      <c r="C26" t="s">
+        <v>80</v>
+      </c>
+      <c r="D26" s="17" t="s">
+        <v>171</v>
+      </c>
+      <c r="E26" s="17" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27">
+        <v>4</v>
+      </c>
+      <c r="B27" t="s">
+        <v>127</v>
+      </c>
+      <c r="C27" t="s">
+        <v>81</v>
+      </c>
+      <c r="D27" s="17" t="s">
+        <v>171</v>
+      </c>
+      <c r="E27" s="17" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28">
+        <v>4</v>
+      </c>
+      <c r="B28" t="s">
+        <v>131</v>
+      </c>
+      <c r="C28" t="s">
+        <v>87</v>
+      </c>
+      <c r="D28" s="17" t="s">
+        <v>191</v>
+      </c>
+      <c r="E28" s="17" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29">
+        <v>4</v>
+      </c>
+      <c r="B29" t="s">
+        <v>145</v>
+      </c>
+      <c r="C29" t="s">
+        <v>213</v>
+      </c>
+      <c r="D29" s="17" t="s">
+        <v>191</v>
+      </c>
+      <c r="E29" s="17" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30">
+        <v>4</v>
+      </c>
+      <c r="B30" t="s">
+        <v>135</v>
+      </c>
+      <c r="C30" t="s">
+        <v>91</v>
+      </c>
+      <c r="D30" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="E30" s="17" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31">
+        <v>4</v>
+      </c>
+      <c r="B31" t="s">
+        <v>139</v>
+      </c>
+      <c r="C31" t="s">
+        <v>95</v>
+      </c>
+      <c r="D31" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="E31" s="17" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32">
+        <v>4</v>
+      </c>
+      <c r="B32" t="s">
+        <v>140</v>
+      </c>
+      <c r="C32" t="s">
+        <v>96</v>
+      </c>
+      <c r="D32" s="17" t="s">
+        <v>190</v>
+      </c>
+      <c r="E32" s="17" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33">
+        <v>4</v>
+      </c>
+      <c r="B33" t="s">
+        <v>141</v>
+      </c>
+      <c r="C33" t="s">
+        <v>106</v>
+      </c>
+      <c r="D33" s="17" t="s">
+        <v>190</v>
+      </c>
+      <c r="E33" s="17" t="s">
+        <v>192</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -3404,10 +3569,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView topLeftCell="A10" zoomScale="150" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75"/>
@@ -3517,6 +3682,27 @@
         <v>19.2</v>
       </c>
     </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="2">
+        <v>41957</v>
+      </c>
+      <c r="B6">
+        <v>8</v>
+      </c>
+      <c r="C6">
+        <v>8</v>
+      </c>
+      <c r="D6">
+        <v>840</v>
+      </c>
+      <c r="E6">
+        <v>200</v>
+      </c>
+      <c r="F6" s="9">
+        <f>(D6-D5)/E6*60</f>
+        <v>142.5</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3530,7 +3716,7 @@
   <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="A2" sqref="A2:B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75"/>
@@ -3585,7 +3771,7 @@
         <v>175</v>
       </c>
       <c r="D2" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="E2">
         <v>15</v>
@@ -3600,7 +3786,7 @@
         <v>90</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -3614,7 +3800,7 @@
         <v>171</v>
       </c>
       <c r="D3" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="E3">
         <v>10</v>
@@ -3629,7 +3815,7 @@
         <v>30</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -3640,10 +3826,10 @@
         <v>62</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
       <c r="D4" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="E4">
         <v>20</v>
@@ -3658,7 +3844,7 @@
         <v>40</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -3669,10 +3855,10 @@
         <v>64</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
       <c r="D5" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="E5">
         <v>40</v>
@@ -3687,7 +3873,7 @@
         <v>10</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -3701,7 +3887,7 @@
         <v>175</v>
       </c>
       <c r="D6" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="E6">
         <v>20</v>
@@ -3716,7 +3902,7 @@
         <v>10</v>
       </c>
       <c r="I6" s="7" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -3727,10 +3913,10 @@
         <v>66</v>
       </c>
       <c r="C7" s="17" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="D7" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="E7">
         <v>30</v>
@@ -3745,7 +3931,7 @@
         <v>15</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -3759,7 +3945,7 @@
         <v>171</v>
       </c>
       <c r="D8" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="E8">
         <v>40</v>
@@ -3774,7 +3960,7 @@
         <v>15</v>
       </c>
       <c r="I8" s="7" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -3785,10 +3971,10 @@
         <v>151</v>
       </c>
       <c r="C9" s="17" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="D9" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="E9">
         <v>30</v>
@@ -3803,37 +3989,37 @@
         <v>20</v>
       </c>
       <c r="I9" s="7" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
     </row>
     <row r="12" spans="1:9">
       <c r="B12" s="5" t="s">
-        <v>211</v>
+        <v>194</v>
       </c>
     </row>
     <row r="13" spans="1:9">
       <c r="B13" s="1" t="s">
-        <v>213</v>
+        <v>196</v>
       </c>
     </row>
     <row r="14" spans="1:9">
       <c r="B14" s="1" t="s">
-        <v>214</v>
+        <v>197</v>
       </c>
     </row>
     <row r="16" spans="1:9">
       <c r="B16" s="1" t="s">
-        <v>212</v>
+        <v>195</v>
       </c>
     </row>
     <row r="17" spans="2:2">
       <c r="B17" s="1" t="s">
-        <v>215</v>
+        <v>198</v>
       </c>
     </row>
     <row r="18" spans="2:2" ht="25.5">
       <c r="B18" s="1" t="s">
-        <v>216</v>
+        <v>199</v>
       </c>
     </row>
   </sheetData>
@@ -3896,7 +4082,7 @@
         <v>171</v>
       </c>
       <c r="D2" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="E2">
         <v>20</v>
@@ -3911,7 +4097,7 @@
         <v>20</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -3925,7 +4111,7 @@
         <v>171</v>
       </c>
       <c r="D3" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="E3">
         <v>40</v>
@@ -3940,7 +4126,7 @@
         <v>10</v>
       </c>
       <c r="I3" s="7" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -3954,7 +4140,7 @@
         <v>175</v>
       </c>
       <c r="D4" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="E4">
         <v>30</v>
@@ -3969,7 +4155,7 @@
         <v>20</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -3983,7 +4169,7 @@
         <v>175</v>
       </c>
       <c r="D5" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="E5">
         <v>25</v>
@@ -3998,7 +4184,7 @@
         <v>25</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -4009,10 +4195,10 @@
         <v>75</v>
       </c>
       <c r="C6" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="D6" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="E6">
         <v>20</v>
@@ -4027,7 +4213,7 @@
         <v>30</v>
       </c>
       <c r="I6" s="7" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -4038,10 +4224,10 @@
         <v>164</v>
       </c>
       <c r="C7" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="D7" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="E7">
         <v>40</v>
@@ -4056,7 +4242,7 @@
         <v>25</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -4067,10 +4253,10 @@
         <v>76</v>
       </c>
       <c r="C8" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
       <c r="D8" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="E8">
         <v>15</v>
@@ -4085,7 +4271,7 @@
         <v>10</v>
       </c>
       <c r="I8" s="7" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -4096,10 +4282,10 @@
         <v>77</v>
       </c>
       <c r="C9" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
       <c r="D9" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="E9">
         <v>15</v>
@@ -4114,32 +4300,32 @@
         <v>15</v>
       </c>
       <c r="I9" s="7" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
     </row>
     <row r="13" spans="1:9">
       <c r="B13" t="s">
-        <v>211</v>
+        <v>194</v>
       </c>
     </row>
     <row r="14" spans="1:9">
       <c r="B14" t="s">
-        <v>226</v>
+        <v>207</v>
       </c>
     </row>
     <row r="15" spans="1:9">
       <c r="B15" t="s">
-        <v>227</v>
+        <v>208</v>
       </c>
     </row>
     <row r="17" spans="2:2">
       <c r="B17" t="s">
-        <v>212</v>
+        <v>195</v>
       </c>
     </row>
     <row r="18" spans="2:2">
       <c r="B18" t="s">
-        <v>228</v>
+        <v>209</v>
       </c>
     </row>
   </sheetData>
@@ -4202,7 +4388,7 @@
         <v>171</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="E2">
         <v>15</v>
@@ -4217,7 +4403,7 @@
         <v>20</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -4231,7 +4417,7 @@
         <v>171</v>
       </c>
       <c r="D3" s="17" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="E3">
         <v>35</v>
@@ -4246,7 +4432,7 @@
         <v>10</v>
       </c>
       <c r="I3" s="7" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -4254,13 +4440,13 @@
         <v>132</v>
       </c>
       <c r="B4" t="s">
-        <v>230</v>
+        <v>211</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="D4" s="17" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="E4">
         <v>20</v>
@@ -4275,7 +4461,7 @@
         <v>20</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -4286,10 +4472,10 @@
         <v>93</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="E5">
         <v>25</v>
@@ -4304,7 +4490,7 @@
         <v>25</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -4318,7 +4504,7 @@
         <v>175</v>
       </c>
       <c r="D6" s="17" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="E6">
         <v>30</v>
@@ -4333,7 +4519,7 @@
         <v>30</v>
       </c>
       <c r="I6" s="7" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -4347,7 +4533,7 @@
         <v>175</v>
       </c>
       <c r="D7" s="17" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="E7">
         <v>20</v>
@@ -4362,7 +4548,7 @@
         <v>25</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -4373,10 +4559,10 @@
         <v>86</v>
       </c>
       <c r="C8" s="17" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
       <c r="D8" s="17" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="E8">
         <v>10</v>
@@ -4391,7 +4577,7 @@
         <v>10</v>
       </c>
       <c r="I8" s="7" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -4399,13 +4585,13 @@
         <v>137</v>
       </c>
       <c r="B9" t="s">
-        <v>231</v>
+        <v>212</v>
       </c>
       <c r="C9" s="17" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
       <c r="D9" s="17" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="E9">
         <v>10</v>
@@ -4420,7 +4606,7 @@
         <v>15</v>
       </c>
       <c r="I9" s="7" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
     </row>
   </sheetData>
@@ -4434,7 +4620,7 @@
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A5" sqref="A5:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75"/>
@@ -4479,10 +4665,10 @@
         <v>80</v>
       </c>
       <c r="C2" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="D2" t="s">
-        <v>229</v>
+        <v>210</v>
       </c>
       <c r="E2">
         <v>20</v>
@@ -4499,10 +4685,10 @@
         <v>81</v>
       </c>
       <c r="C3" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="D3" t="s">
-        <v>229</v>
+        <v>210</v>
       </c>
       <c r="E3">
         <v>35</v>
@@ -4522,7 +4708,7 @@
         <v>171</v>
       </c>
       <c r="D4" t="s">
-        <v>229</v>
+        <v>210</v>
       </c>
       <c r="E4">
         <v>20</v>
@@ -4533,16 +4719,16 @@
     </row>
     <row r="5" spans="1:9">
       <c r="A5" t="s">
-        <v>133</v>
+        <v>145</v>
       </c>
       <c r="B5" t="s">
-        <v>89</v>
+        <v>213</v>
       </c>
       <c r="C5" t="s">
         <v>171</v>
       </c>
       <c r="D5" t="s">
-        <v>229</v>
+        <v>210</v>
       </c>
       <c r="E5">
         <v>35</v>
@@ -4562,7 +4748,7 @@
         <v>175</v>
       </c>
       <c r="D6" t="s">
-        <v>229</v>
+        <v>210</v>
       </c>
       <c r="E6">
         <v>30</v>
@@ -4582,7 +4768,7 @@
         <v>175</v>
       </c>
       <c r="D7" t="s">
-        <v>229</v>
+        <v>210</v>
       </c>
       <c r="E7">
         <v>25</v>
@@ -4599,10 +4785,10 @@
         <v>96</v>
       </c>
       <c r="C8" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
       <c r="D8" t="s">
-        <v>229</v>
+        <v>210</v>
       </c>
       <c r="E8">
         <v>15</v>
@@ -4619,10 +4805,10 @@
         <v>106</v>
       </c>
       <c r="C9" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
       <c r="D9" t="s">
-        <v>229</v>
+        <v>210</v>
       </c>
       <c r="E9">
         <v>10</v>
@@ -4641,8 +4827,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75"/>
@@ -4802,7 +4988,7 @@
         <v>75</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>222</v>
+        <v>205</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="31.5">
@@ -4813,7 +4999,7 @@
         <v>164</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>224</v>
+        <v>206</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="15.75">

</xml_diff>